<commit_message>
Added functional healthbar slider
</commit_message>
<xml_diff>
--- a/TeamProj/To Do List.xlsx
+++ b/TeamProj/To Do List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitHub\GameDev\TeamProj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BFB4FD6A-B6F2-4516-8D6A-B35A47530DB4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D75241FA-CEDB-4F22-817C-FFE6D9E9133A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="16560" windowHeight="6108" xr2:uid="{84DFA9FA-86F3-4D98-8434-FAAA3191E55F}"/>
+    <workbookView xWindow="1872" yWindow="0" windowWidth="16560" windowHeight="6108" xr2:uid="{84DFA9FA-86F3-4D98-8434-FAAA3191E55F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Cole</t>
   </si>
@@ -80,10 +80,7 @@
     <t>Player getting through the dashable walls</t>
   </si>
   <si>
-    <t xml:space="preserve">Player dash </t>
-  </si>
-  <si>
-    <t>Add, test, finalize dash animation</t>
+    <t>Add, test, finalize dash and animation</t>
   </si>
 </sst>
 </file>
@@ -484,7 +481,7 @@
   <dimension ref="A3:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,9 +554,6 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>

</xml_diff>